<commit_message>
Updated output files added
</commit_message>
<xml_diff>
--- a/MicrosoftTeamsAttendance/processed_attendance.xlsx
+++ b/MicrosoftTeamsAttendance/processed_attendance.xlsx
@@ -1084,559 +1084,559 @@
     <t>9217TZY2307</t>
   </si>
   <si>
-    <t>( 11:13:06 AM,  12:24:55 PM, 1:11:49)</t>
-  </si>
-  <si>
-    <t>( 10:57:43 AM,  10:59:07 AM, 0:01:24)( 10:59:07 AM,  12:24:29 PM, 1:25:22)</t>
-  </si>
-  <si>
-    <t>( 11:02:50 AM,  11:03:01 AM, 0:00:11)</t>
-  </si>
-  <si>
-    <t>( 10:59:06 AM,  12:03:49 PM, 1:04:43)</t>
-  </si>
-  <si>
-    <t>( 11:16:00 AM,  12:30:00 PM, 1:14:00)</t>
-  </si>
-  <si>
-    <t>( 10:56:12 AM,  10:59:05 AM, 0:02:53)( 10:59:06 AM,  12:25:03 PM, 1:25:57)</t>
-  </si>
-  <si>
-    <t>( 11:04:03 AM,  11:38:12 AM, 0:34:09)( 11:51:34 AM,  12:09:48 PM, 0:18:14)( 12:18:24 PM,  12:25:10 PM, 0:06:46)</t>
-  </si>
-  <si>
-    <t>( 10:56:12 AM,  10:57:27 AM, 0:01:15)( 10:57:47 AM,  10:59:05 AM, 0:01:18)( 10:59:06 AM,  11:13:19 AM, 0:14:13)</t>
-  </si>
-  <si>
-    <t>( 11:12:16 AM,  12:30:00 PM, 1:17:44)</t>
-  </si>
-  <si>
-    <t>( 11:07:27 AM,  12:24:57 PM, 1:17:30)</t>
-  </si>
-  <si>
-    <t>( 10:57:43 AM,  10:57:57 AM, 0:00:14)( 10:58:14 AM,  10:58:18 AM, 0:00:04)( 10:59:29 AM,  12:25:08 PM, 1:25:39)</t>
-  </si>
-  <si>
-    <t>( 10:59:39 AM,  12:24:43 PM, 1:25:04)</t>
-  </si>
-  <si>
-    <t>( 10:56:12 AM,  11:05:05 AM, 0:08:53)( 11:03:54 AM,  12:24:36 PM, 1:20:42)</t>
-  </si>
-  <si>
-    <t>( 11:18:06 AM,  11:23:05 AM, 0:04:59)( 11:29:12 AM,  11:33:57 AM, 0:04:45)</t>
-  </si>
-  <si>
-    <t>( 11:02:04 AM,  12:24:44 PM, 1:22:40)</t>
-  </si>
-  <si>
-    <t>( 11:07:35 AM,  11:20:47 AM, 0:13:12)</t>
-  </si>
-  <si>
-    <t>( 11:00:36 AM,  11:00:46 AM, 0:00:10)( 11:01:10 AM,  12:25:07 PM, 1:23:57)</t>
-  </si>
-  <si>
-    <t>( 11:00:30 AM,  11:01:14 AM, 0:00:44)( 11:01:14 AM,  12:25:05 PM, 1:23:51)</t>
-  </si>
-  <si>
-    <t>( 11:01:38 AM,  12:25:28 PM, 1:23:50)</t>
-  </si>
-  <si>
-    <t>( 11:06:54 AM,  12:26:56 PM, 1:20:02)</t>
-  </si>
-  <si>
-    <t>( 11:00:34 AM,  11:00:37 AM, 0:00:03)</t>
-  </si>
-  <si>
-    <t>( 11:10:48 AM,  11:14:27 AM, 0:03:39)</t>
-  </si>
-  <si>
-    <t>( 11:08:13 AM,  12:03:57 PM, 0:55:44)</t>
-  </si>
-  <si>
-    <t>( 11:10:25 AM,  12:25:46 PM, 1:15:21)</t>
-  </si>
-  <si>
-    <t>( 11:01:13 AM,  12:24:31 PM, 1:23:18)</t>
-  </si>
-  <si>
-    <t>( 11:37:48 AM,  12:02:10 PM, 0:24:22)</t>
-  </si>
-  <si>
-    <t>( 11:21:57 AM,  12:25:38 PM, 1:03:41)</t>
-  </si>
-  <si>
-    <t>( 11:03:14 AM,  12:24:55 PM, 1:21:41)</t>
-  </si>
-  <si>
-    <t>( 11:02:14 AM,  12:24:51 PM, 1:22:37)</t>
-  </si>
-  <si>
-    <t>( 10:58:20 AM,  11:01:23 AM, 0:03:03)</t>
-  </si>
-  <si>
-    <t>( 11:39:54 AM,  12:02:22 PM, 0:22:28)</t>
-  </si>
-  <si>
-    <t>( 11:11:32 AM,  11:13:41 AM, 0:02:09)( 11:13:57 AM,  11:14:05 AM, 0:00:08)( 11:18:32 AM,  11:20:49 AM, 0:02:17)( 11:22:47 AM,  12:25:32 PM, 1:02:45)</t>
-  </si>
-  <si>
-    <t>( 10:56:12 AM,  10:56:32 AM, 0:00:20)</t>
-  </si>
-  <si>
-    <t>( 11:00:24 AM,  12:11:53 PM, 1:11:29)</t>
-  </si>
-  <si>
-    <t>( 10:57:09 AM,  10:59:33 AM, 0:02:24)</t>
-  </si>
-  <si>
-    <t>( 10:56:12 AM,  10:59:06 AM, 0:02:54)( 10:59:06 AM,  12:24:54 PM, 1:25:48)</t>
-  </si>
-  <si>
-    <t>( 10:57:23 AM,  10:59:05 AM, 0:01:42)( 10:59:06 AM,  12:25:05 PM, 1:25:59)</t>
-  </si>
-  <si>
-    <t>( 11:50:25 AM,  11:51:45 AM, 0:01:20)</t>
-  </si>
-  <si>
-    <t>( 11:00:06 AM,  11:00:23 AM, 0:00:17)</t>
-  </si>
-  <si>
-    <t>( 11:00:03 AM,  12:19:15 PM, 1:19:12)</t>
-  </si>
-  <si>
-    <t>( 11:00:56 AM,  11:01:00 AM, 0:00:04)( 11:01:10 AM,  11:07:54 AM, 0:06:44)( 11:10:56 AM,  11:13:12 AM, 0:02:16)</t>
-  </si>
-  <si>
-    <t>( 10:56:12 AM,  12:25:04 PM, 1:28:52)( 12:26:13 PM,  12:26:30 PM, 0:00:17)</t>
-  </si>
-  <si>
-    <t>( 10:57:54 AM,  10:58:13 AM, 0:00:19)( 10:58:20 AM,  10:59:05 AM, 0:00:45)( 10:59:06 AM,  12:25:01 PM, 1:25:55)</t>
-  </si>
-  <si>
-    <t>( 10:56:12 AM,  10:56:18 AM, 0:00:06)( 10:56:27 AM,  10:57:22 AM, 0:00:55)( 10:58:30 AM,  10:59:04 AM, 0:00:34)( 10:59:05 AM,  12:25:02 PM, 1:25:57)</t>
-  </si>
-  <si>
-    <t>( 11:03:18 AM,  11:03:24 AM, 0:00:06)( 11:03:24 AM,  11:32:11 AM, 0:28:47)( 11:36:23 AM,  12:05:40 PM, 0:29:17)( 12:05:51 PM,  12:25:01 PM, 0:19:10)</t>
-  </si>
-  <si>
-    <t>( 11:06:47 AM,  12:25:04 PM, 1:18:17)</t>
-  </si>
-  <si>
-    <t>( 11:04:20 AM,  11:05:16 AM, 0:00:56)</t>
-  </si>
-  <si>
-    <t>( 11:00:26 AM,  11:01:14 AM, 0:00:48)( 11:01:15 AM,  12:16:41 PM, 1:15:26)</t>
-  </si>
-  <si>
-    <t>( 11:00:03 AM,  12:30:00 PM, 1:29:57)</t>
-  </si>
-  <si>
-    <t>( 11:01:42 AM,  11:02:18 AM, 0:00:36)( 11:03:42 AM,  11:41:47 AM, 0:38:05)</t>
-  </si>
-  <si>
-    <t>( 11:08:36 AM,  11:21:07 AM, 0:12:31)</t>
-  </si>
-  <si>
-    <t>( 11:42:16 AM,  12:25:13 PM, 0:42:57)</t>
-  </si>
-  <si>
-    <t>( 12:13:37 PM,  12:30:00 PM, 0:16:23)</t>
-  </si>
-  <si>
-    <t>( 11:24:22 AM,  11:26:31 AM, 0:02:09)</t>
-  </si>
-  <si>
-    <t>( 11:16:24 AM,  12:30:00 PM, 1:13:36)</t>
-  </si>
-  <si>
-    <t>( 11:01:15 AM,  11:01:32 AM, 0:00:17)( 11:01:32 AM,  12:24:32 PM, 1:23:00)</t>
-  </si>
-  <si>
-    <t>( 11:59:35 AM,  12:02:09 PM, 0:02:34)( 12:02:53 PM,  12:30:00 PM, 0:27:07)</t>
-  </si>
-  <si>
-    <t>( 10:59:29 AM,  11:02:18 AM, 0:02:49)( 11:17:23 AM,  12:25:50 PM, 1:08:27)</t>
-  </si>
-  <si>
-    <t>( 10:56:32 AM,  10:59:04 AM, 0:02:32)( 10:59:05 AM,  12:25:13 PM, 1:26:08)</t>
-  </si>
-  <si>
-    <t>( 11:07:05 AM,  12:01:45 PM, 0:54:40)</t>
-  </si>
-  <si>
-    <t>( 10:58:54 AM,  10:59:04 AM, 0:00:10)( 10:59:05 AM,  12:18:38 PM, 1:19:33)( 12:22:20 PM,  12:30:00 PM, 0:07:40)</t>
-  </si>
-  <si>
-    <t>( 10:57:44 AM,  10:59:04 AM, 0:01:20)( 10:59:06 AM,  11:36:12 AM, 0:37:06)( 11:37:03 AM,  12:26:07 PM, 0:49:04)</t>
-  </si>
-  <si>
-    <t>( 11:12:09 AM,  11:36:04 AM, 0:23:55)</t>
-  </si>
-  <si>
-    <t>( 11:01:23 AM,  12:30:00 PM, 1:28:37)</t>
-  </si>
-  <si>
-    <t>( 10:57:51 AM,  10:58:22 AM, 0:00:31)( 10:58:57 AM,  10:59:03 AM, 0:00:06)( 10:59:05 AM,  12:25:48 PM, 1:26:43)</t>
-  </si>
-  <si>
-    <t>( 11:01:42 AM,  11:01:49 AM, 0:00:07)( 11:03:06 AM,  11:03:13 AM, 0:00:07)( 11:04:26 AM,  11:31:12 AM, 0:26:46)( 11:32:21 AM,  12:21:46 PM, 0:49:25)</t>
-  </si>
-  <si>
-    <t>( 11:08:35 AM,  12:24:27 PM, 1:15:52)</t>
-  </si>
-  <si>
-    <t>( 11:00:01 AM,  11:00:06 AM, 0:00:05)( 11:00:22 AM,  12:25:36 PM, 1:25:14)</t>
-  </si>
-  <si>
-    <t>( 11:50:48 AM,  12:13:12 PM, 0:22:24)</t>
-  </si>
-  <si>
-    <t>( 10:56:12 AM,  10:56:16 AM, 0:00:04)( 11:01:29 AM,  11:01:37 AM, 0:00:08)( 11:03:05 AM,  11:03:11 AM, 0:00:06)( 11:15:20 AM,  12:16:00 PM, 1:00:40)</t>
-  </si>
-  <si>
-    <t>( 11:00:09 AM,  11:02:57 AM, 0:02:48)( 11:03:32 AM,  12:25:07 PM, 1:21:35)</t>
-  </si>
-  <si>
-    <t>( 11:51:10 AM,  12:24:55 PM, 0:33:45)</t>
-  </si>
-  <si>
-    <t>( 11:11:17 AM,  12:04:07 PM, 0:52:50)</t>
-  </si>
-  <si>
-    <t>( 11:07:51 AM,  12:25:13 PM, 1:17:22)</t>
-  </si>
-  <si>
-    <t>( 11:00:14 AM,  12:30:00 PM, 1:29:46)</t>
-  </si>
-  <si>
-    <t>( 11:16:55 AM,  11:48:32 AM, 0:31:37)( 11:48:46 AM,  11:49:33 AM, 0:00:47)</t>
-  </si>
-  <si>
-    <t>( 10:56:12 AM,  10:56:34 AM, 0:00:22)</t>
-  </si>
-  <si>
-    <t>( 11:02:03 AM,  12:30:00 PM, 1:27:57)</t>
-  </si>
-  <si>
-    <t>( 11:04:31 AM,  11:04:45 AM, 0:00:14)</t>
-  </si>
-  <si>
-    <t>( 10:57:08 AM,  10:59:05 AM, 0:01:57)( 10:59:05 AM,  12:21:52 PM, 1:22:47)</t>
-  </si>
-  <si>
-    <t>( 11:05:59 AM,  11:06:25 AM, 0:00:26)( 11:06:40 AM,  11:51:48 AM, 0:45:08)( 11:57:55 AM,  12:30:00 PM, 0:32:05)</t>
-  </si>
-  <si>
-    <t>( 12:21:14 PM,  12:25:10 PM, 0:03:56)</t>
-  </si>
-  <si>
-    <t>( 10:57:44 AM,  10:59:04 AM, 0:01:20)( 10:59:04 AM,  11:55:52 AM, 0:56:48)( 11:59:19 AM,  12:24:53 PM, 0:25:34)</t>
-  </si>
-  <si>
-    <t>( 11:32:42 AM,  12:24:26 PM, 0:51:44)</t>
-  </si>
-  <si>
-    <t>( 11:06:32 AM,  11:23:56 AM, 0:17:24)</t>
-  </si>
-  <si>
-    <t>( 11:02:11 AM,  12:30:00 PM, 1:27:49)</t>
-  </si>
-  <si>
-    <t>( 11:01:49 AM,  11:01:58 AM, 0:00:09)( 11:01:58 AM,  11:03:24 AM, 0:01:26)( 11:03:28 AM,  12:25:03 PM, 1:21:35)</t>
-  </si>
-  <si>
-    <t>( 11:31:47 AM,  11:41:58 AM, 0:10:11)( 11:59:31 AM,  12:04:22 PM, 0:04:51)</t>
-  </si>
-  <si>
-    <t>( 10:59:31 AM,  12:25:00 PM, 1:25:29)</t>
-  </si>
-  <si>
-    <t>( 11:00:46 AM,  12:24:38 PM, 1:23:52)</t>
-  </si>
-  <si>
-    <t>( 11:11:15 AM,  12:30:00 PM, 1:18:45)</t>
-  </si>
-  <si>
-    <t>( 11:01:01 AM,  11:01:13 AM, 0:00:12)( 11:01:13 AM,  12:24:29 PM, 1:23:16)</t>
-  </si>
-  <si>
-    <t>( 11:16:33 AM,  11:18:41 AM, 0:02:08)</t>
-  </si>
-  <si>
-    <t>( 11:00:22 AM,  12:24:41 PM, 1:24:19)</t>
-  </si>
-  <si>
-    <t>( 10:59:19 AM,  12:24:23 PM, 1:25:04)</t>
-  </si>
-  <si>
-    <t>( 11:00:31 AM,  11:47:23 AM, 0:46:52)</t>
-  </si>
-  <si>
-    <t>( 10:56:12 AM,  10:59:03 AM, 0:02:51)( 10:57:29 AM,  10:59:05 AM, 0:01:36)( 10:59:04 AM,  11:37:00 AM, 0:37:56)( 10:59:06 AM,  12:25:18 PM, 1:26:12)</t>
-  </si>
-  <si>
-    <t>( 10:56:12 AM,  12:25:15 PM, 1:29:03)</t>
-  </si>
-  <si>
-    <t>( 11:06:11 AM,  12:05:09 PM, 0:58:58)</t>
-  </si>
-  <si>
-    <t>( 11:01:34 AM,  11:12:49 AM, 0:11:15)</t>
-  </si>
-  <si>
-    <t>( 11:45:23 AM,  12:25:08 PM, 0:39:45)</t>
-  </si>
-  <si>
-    <t>( 11:00:09 AM,  12:25:02 PM, 1:24:53)</t>
-  </si>
-  <si>
-    <t>( 10:56:14 AM,  10:56:21 AM, 0:00:07)( 10:59:45 AM,  11:00:21 AM, 0:00:36)</t>
-  </si>
-  <si>
-    <t>( 11:00:37 AM,  11:01:15 AM, 0:00:38)( 11:01:15 AM,  11:23:00 AM, 0:21:45)( 12:12:13 PM,  12:22:38 PM, 0:10:25)</t>
-  </si>
-  <si>
-    <t>( 11:02:06 AM,  12:25:00 PM, 1:22:54)</t>
-  </si>
-  <si>
-    <t>( 11:19:57 AM,  11:21:25 AM, 0:01:28)( 11:24:00 AM,  12:25:03 PM, 1:01:03)</t>
-  </si>
-  <si>
-    <t>( 10:56:14 AM,  10:59:06 AM, 0:02:52)( 10:59:07 AM,  11:59:05 AM, 0:59:58)</t>
-  </si>
-  <si>
-    <t>( 10:59:53 AM,  12:25:04 PM, 1:25:11)</t>
-  </si>
-  <si>
-    <t>( 11:02:49 AM,  11:03:24 AM, 0:00:35)( 11:03:24 AM,  12:24:58 PM, 1:21:34)</t>
-  </si>
-  <si>
-    <t>( 10:57:56 AM,  10:59:07 AM, 0:01:11)( 10:59:07 AM,  12:24:36 PM, 1:25:29)( 11:34:46 AM,  12:27:15 PM, 0:52:29)</t>
-  </si>
-  <si>
-    <t>( 10:57:39 AM,  10:59:07 AM, 0:01:28)( 10:59:07 AM,  12:24:36 PM, 1:25:29)</t>
-  </si>
-  <si>
-    <t>( 11:21:29 AM,  12:24:58 PM, 1:03:29)</t>
-  </si>
-  <si>
-    <t>( 10:59:25 AM,  12:17:44 PM, 1:18:19)</t>
-  </si>
-  <si>
-    <t>( 11:02:34 AM,  11:34:36 AM, 0:32:02)( 11:35:02 AM,  12:25:04 PM, 0:50:02)</t>
-  </si>
-  <si>
-    <t>( 11:26:42 AM,  12:25:05 PM, 0:58:23)</t>
-  </si>
-  <si>
-    <t>( 11:00:44 AM,  11:01:14 AM, 0:00:30)( 11:01:14 AM,  11:21:55 AM, 0:20:41)</t>
-  </si>
-  <si>
-    <t>( 11:04:26 AM,  11:04:35 AM, 0:00:09)</t>
-  </si>
-  <si>
-    <t>( 11:02:49 AM,  12:24:58 PM, 1:22:09)</t>
-  </si>
-  <si>
-    <t>( 11:05:04 AM,  11:05:46 AM, 0:00:42)( 11:05:46 AM,  12:30:00 PM, 1:24:14)</t>
-  </si>
-  <si>
-    <t>( 11:20:41 AM,  11:23:17 AM, 0:02:36)</t>
-  </si>
-  <si>
-    <t>( 10:59:13 AM,  10:59:21 AM, 0:00:08)</t>
-  </si>
-  <si>
-    <t>( 11:24:21 AM,  12:24:59 PM, 1:00:38)</t>
-  </si>
-  <si>
-    <t>( 10:58:03 AM,  10:58:08 AM, 0:00:05)( 10:59:07 AM,  12:24:52 PM, 1:25:45)</t>
-  </si>
-  <si>
-    <t>( 11:32:38 AM,  12:25:02 PM, 0:52:24)</t>
-  </si>
-  <si>
-    <t>( 10:56:12 AM,  10:57:10 AM, 0:00:58)( 11:00:13 AM,  12:14:51 PM, 1:14:38)( 12:16:25 PM,  12:30:00 PM, 0:13:35)</t>
-  </si>
-  <si>
-    <t>( 11:08:45 AM,  11:14:40 AM, 0:05:55)</t>
-  </si>
-  <si>
-    <t>( 10:58:43 AM,  10:59:04 AM, 0:00:21)( 10:59:05 AM,  12:25:10 PM, 1:26:05)</t>
-  </si>
-  <si>
-    <t>( 11:35:43 AM,  12:23:35 PM, 0:47:52)</t>
-  </si>
-  <si>
-    <t>( 11:13:09 AM,  11:50:42 AM, 0:37:33)</t>
-  </si>
-  <si>
-    <t>( 10:57:37 AM,  10:59:03 AM, 0:01:26)( 10:59:04 AM,  12:30:00 PM, 1:30:56)</t>
-  </si>
-  <si>
-    <t>( 11:02:33 AM,  12:24:56 PM, 1:22:23)</t>
-  </si>
-  <si>
-    <t>( 11:00:51 AM,  12:25:04 PM, 1:24:13)</t>
-  </si>
-  <si>
-    <t>( 11:06:52 AM,  12:25:05 PM, 1:18:13)</t>
-  </si>
-  <si>
-    <t>( 10:57:47 AM,  10:58:09 AM, 0:00:22)</t>
-  </si>
-  <si>
-    <t>( 11:01:49 AM,  11:37:50 AM, 0:36:01)( 11:38:00 AM,  12:16:12 PM, 0:38:12)( 12:17:57 PM,  12:25:14 PM, 0:07:17)</t>
-  </si>
-  <si>
-    <t>( 11:09:46 AM,  11:46:00 AM, 0:36:14)( 11:46:14 AM,  12:25:16 PM, 0:39:02)</t>
-  </si>
-  <si>
-    <t>( 11:05:06 AM,  12:24:57 PM, 1:19:51)</t>
-  </si>
-  <si>
-    <t>( 10:58:49 AM,  10:59:05 AM, 0:00:16)</t>
-  </si>
-  <si>
-    <t>( 11:13:00 AM,  11:15:15 AM, 0:02:15)</t>
-  </si>
-  <si>
-    <t>( 12:22:04 PM,  12:24:57 PM, 0:02:53)</t>
-  </si>
-  <si>
-    <t>( 11:01:57 AM,  11:37:08 AM, 0:35:11)</t>
-  </si>
-  <si>
-    <t>( 11:08:28 AM,  12:24:45 PM, 1:16:17)</t>
-  </si>
-  <si>
-    <t>( 11:07:24 AM,  11:56:41 AM, 0:49:17)</t>
-  </si>
-  <si>
-    <t>( 11:02:14 AM,  12:25:03 PM, 1:22:49)</t>
-  </si>
-  <si>
-    <t>( 11:00:01 AM,  11:05:38 AM, 0:05:37)</t>
-  </si>
-  <si>
-    <t>( 10:56:12 AM,  12:25:05 PM, 1:28:53)</t>
-  </si>
-  <si>
-    <t>( 11:00:27 AM,  11:01:14 AM, 0:00:47)( 11:01:14 AM,  12:25:06 PM, 1:23:52)</t>
-  </si>
-  <si>
-    <t>( 11:07:16 AM,  11:15:45 AM, 0:08:29)( 11:16:35 AM,  12:25:01 PM, 1:08:26)</t>
-  </si>
-  <si>
-    <t>( 11:40:22 AM,  11:41:35 AM, 0:01:13)</t>
-  </si>
-  <si>
-    <t>( 11:01:33 AM,  12:03:59 PM, 1:02:26)</t>
-  </si>
-  <si>
-    <t>( 11:00:08 AM,  12:27:30 PM, 1:27:22)</t>
-  </si>
-  <si>
-    <t>( 11:01:47 AM,  12:24:35 PM, 1:22:48)</t>
-  </si>
-  <si>
-    <t>( 10:56:53 AM,  10:57:01 AM, 0:00:08)( 10:57:07 AM,  10:59:05 AM, 0:01:58)( 10:58:40 AM,  10:59:05 AM, 0:00:25)( 10:59:06 AM,  11:00:25 AM, 0:01:19)( 11:01:08 AM,  12:26:59 PM, 1:25:51)</t>
-  </si>
-  <si>
-    <t>( 10:58:27 AM,  10:58:52 AM, 0:00:25)( 11:00:32 AM,  12:30:00 PM, 1:29:28)</t>
-  </si>
-  <si>
-    <t>( 11:15:27 AM,  12:25:13 PM, 1:09:46)</t>
-  </si>
-  <si>
-    <t>( 10:56:16 AM,  10:59:05 AM, 0:02:49)( 10:59:06 AM,  12:24:58 PM, 1:25:52)</t>
-  </si>
-  <si>
-    <t>( 11:03:01 AM,  12:26:57 PM, 1:23:56)</t>
-  </si>
-  <si>
-    <t>( 10:58:58 AM,  10:59:33 AM, 0:00:35)( 11:00:30 AM,  12:03:51 PM, 1:03:21)</t>
-  </si>
-  <si>
-    <t>( 11:14:25 AM,  11:20:25 AM, 0:06:00)</t>
-  </si>
-  <si>
-    <t>( 11:03:40 AM,  12:14:23 PM, 1:10:43)( 12:14:30 PM,  12:25:04 PM, 0:10:34)</t>
-  </si>
-  <si>
-    <t>( 10:59:47 AM,  11:00:02 AM, 0:00:15)( 11:00:02 AM,  12:25:12 PM, 1:25:10)</t>
-  </si>
-  <si>
-    <t>( 11:11:30 AM,  12:09:29 PM, 0:57:59)</t>
-  </si>
-  <si>
-    <t>( 11:07:40 AM,  12:30:00 PM, 1:22:20)</t>
-  </si>
-  <si>
-    <t>( 11:00:05 AM,  12:15:24 PM, 1:15:19)</t>
-  </si>
-  <si>
-    <t>( 10:58:08 AM,  10:59:05 AM, 0:00:57)( 10:59:06 AM,  12:24:29 PM, 1:25:23)</t>
-  </si>
-  <si>
-    <t>( 11:10:35 AM,  12:25:16 PM, 1:14:41)</t>
-  </si>
-  <si>
-    <t>( 11:04:00 AM,  11:04:13 AM, 0:00:13)</t>
-  </si>
-  <si>
-    <t>( 10:59:12 AM,  11:16:55 AM, 0:17:43)( 11:17:42 AM,  12:24:01 PM, 1:06:19)</t>
-  </si>
-  <si>
-    <t>( 11:27:38 AM,  11:28:47 AM, 0:01:09)( 11:30:34 AM,  11:44:52 AM, 0:14:18)</t>
-  </si>
-  <si>
-    <t>( 11:02:43 AM,  11:02:59 AM, 0:00:16)( 11:03:19 AM,  12:25:01 PM, 1:21:42)</t>
-  </si>
-  <si>
-    <t>( 11:55:42 AM,  11:58:13 AM, 0:02:31)</t>
-  </si>
-  <si>
-    <t>( 11:04:42 AM,  11:04:59 AM, 0:00:17)( 11:04:59 AM,  11:05:34 AM, 0:00:35)( 11:07:32 AM,  11:12:04 AM, 0:04:32)</t>
-  </si>
-  <si>
-    <t>( 11:05:07 AM,  11:14:35 AM, 0:09:28)</t>
-  </si>
-  <si>
-    <t>( 11:16:44 AM,  11:45:33 AM, 0:28:49)</t>
-  </si>
-  <si>
-    <t>( 10:56:12 AM,  12:25:10 PM, 1:28:58)</t>
-  </si>
-  <si>
-    <t>( 10:56:19 AM,  12:25:34 PM, 1:29:15)</t>
-  </si>
-  <si>
-    <t>( 11:03:54 AM,  12:23:36 PM, 1:19:42)</t>
-  </si>
-  <si>
-    <t>( 11:56:03 AM,  12:06:08 PM, 0:10:05)</t>
-  </si>
-  <si>
-    <t>( 11:00:47 AM,  11:01:11 AM, 0:00:24)</t>
-  </si>
-  <si>
-    <t>( 11:12:32 AM,  12:03:03 PM, 0:50:31)( 12:04:41 PM,  12:11:01 PM, 0:06:20)</t>
-  </si>
-  <si>
-    <t>( 11:01:03 AM,  11:05:09 AM, 0:04:06)( 11:05:12 AM,  11:07:02 AM, 0:01:50)</t>
-  </si>
-  <si>
-    <t>( 11:45:53 AM,  11:48:00 AM, 0:02:07)</t>
-  </si>
-  <si>
-    <t>( 11:01:44 AM,  12:16:50 PM, 1:15:06)</t>
-  </si>
-  <si>
-    <t>( 11:07:04 AM,  12:24:40 PM, 1:17:36)</t>
-  </si>
-  <si>
-    <t>( 11:01:17 AM,  11:03:05 AM, 0:01:48)( 11:02:50 AM,  11:03:22 AM, 0:00:32)( 11:03:22 AM,  11:07:12 AM, 0:03:50)( 11:06:27 AM,  12:15:03 PM, 1:08:36)( 12:13:07 PM,  12:25:08 PM, 0:12:01)</t>
+    <t xml:space="preserve">(  11:13:06 AM,  12:24:55 PM, 1:11:49) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  10:57:43 AM,  10:59:07 AM, 0:01:24) \n (  10:59:07 AM,  12:24:29 PM, 1:25:22) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:02:50 AM,  11:03:01 AM, 0:00:11) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  10:59:06 AM,  12:03:49 PM, 1:04:43) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:16:00 AM,  12:30:00 PM, 1:14:00) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  10:56:12 AM,  10:59:05 AM, 0:02:53) \n (  10:59:06 AM,  12:25:03 PM, 1:25:57) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:04:03 AM,  11:38:12 AM, 0:34:09) \n (  11:51:34 AM,  12:09:48 PM, 0:18:14) \n (  12:18:24 PM,  12:25:10 PM, 0:06:46) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  10:56:12 AM,  10:57:27 AM, 0:01:15) \n (  10:57:47 AM,  10:59:05 AM, 0:01:18) \n (  10:59:06 AM,  11:13:19 AM, 0:14:13) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:12:16 AM,  12:30:00 PM, 1:17:44) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:07:27 AM,  12:24:57 PM, 1:17:30) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  10:57:43 AM,  10:57:57 AM, 0:00:14) \n (  10:58:14 AM,  10:58:18 AM, 0:00:04) \n (  10:59:29 AM,  12:25:08 PM, 1:25:39) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  10:59:39 AM,  12:24:43 PM, 1:25:04) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  10:56:12 AM,  11:05:05 AM, 0:08:53) \n (  11:03:54 AM,  12:24:36 PM, 1:20:42) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:18:06 AM,  11:23:05 AM, 0:04:59) \n (  11:29:12 AM,  11:33:57 AM, 0:04:45) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:02:04 AM,  12:24:44 PM, 1:22:40) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:07:35 AM,  11:20:47 AM, 0:13:12) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:00:36 AM,  11:00:46 AM, 0:00:10) \n (  11:01:10 AM,  12:25:07 PM, 1:23:57) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:00:30 AM,  11:01:14 AM, 0:00:44) \n (  11:01:14 AM,  12:25:05 PM, 1:23:51) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:01:38 AM,  12:25:28 PM, 1:23:50) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:06:54 AM,  12:26:56 PM, 1:20:02) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:00:34 AM,  11:00:37 AM, 0:00:03) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:10:48 AM,  11:14:27 AM, 0:03:39) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:08:13 AM,  12:03:57 PM, 0:55:44) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:10:25 AM,  12:25:46 PM, 1:15:21) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:01:13 AM,  12:24:31 PM, 1:23:18) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:37:48 AM,  12:02:10 PM, 0:24:22) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:21:57 AM,  12:25:38 PM, 1:03:41) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:03:14 AM,  12:24:55 PM, 1:21:41) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:02:14 AM,  12:24:51 PM, 1:22:37) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  10:58:20 AM,  11:01:23 AM, 0:03:03) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:39:54 AM,  12:02:22 PM, 0:22:28) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:11:32 AM,  11:13:41 AM, 0:02:09) \n (  11:13:57 AM,  11:14:05 AM, 0:00:08) \n (  11:18:32 AM,  11:20:49 AM, 0:02:17) \n (  11:22:47 AM,  12:25:32 PM, 1:02:45) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  10:56:12 AM,  10:56:32 AM, 0:00:20) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:00:24 AM,  12:11:53 PM, 1:11:29) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  10:57:09 AM,  10:59:33 AM, 0:02:24) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  10:56:12 AM,  10:59:06 AM, 0:02:54) \n (  10:59:06 AM,  12:24:54 PM, 1:25:48) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  10:57:23 AM,  10:59:05 AM, 0:01:42) \n (  10:59:06 AM,  12:25:05 PM, 1:25:59) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:50:25 AM,  11:51:45 AM, 0:01:20) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:00:06 AM,  11:00:23 AM, 0:00:17) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:00:03 AM,  12:19:15 PM, 1:19:12) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:00:56 AM,  11:01:00 AM, 0:00:04) \n (  11:01:10 AM,  11:07:54 AM, 0:06:44) \n (  11:10:56 AM,  11:13:12 AM, 0:02:16) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  10:56:12 AM,  12:25:04 PM, 1:28:52) \n (  12:26:13 PM,  12:26:30 PM, 0:00:17) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  10:57:54 AM,  10:58:13 AM, 0:00:19) \n (  10:58:20 AM,  10:59:05 AM, 0:00:45) \n (  10:59:06 AM,  12:25:01 PM, 1:25:55) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  10:56:12 AM,  10:56:18 AM, 0:00:06) \n (  10:56:27 AM,  10:57:22 AM, 0:00:55) \n (  10:58:30 AM,  10:59:04 AM, 0:00:34) \n (  10:59:05 AM,  12:25:02 PM, 1:25:57) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:03:18 AM,  11:03:24 AM, 0:00:06) \n (  11:03:24 AM,  11:32:11 AM, 0:28:47) \n (  11:36:23 AM,  12:05:40 PM, 0:29:17) \n (  12:05:51 PM,  12:25:01 PM, 0:19:10) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:06:47 AM,  12:25:04 PM, 1:18:17) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:04:20 AM,  11:05:16 AM, 0:00:56) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:00:26 AM,  11:01:14 AM, 0:00:48) \n (  11:01:15 AM,  12:16:41 PM, 1:15:26) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:00:03 AM,  12:30:00 PM, 1:29:57) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:01:42 AM,  11:02:18 AM, 0:00:36) \n (  11:03:42 AM,  11:41:47 AM, 0:38:05) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:08:36 AM,  11:21:07 AM, 0:12:31) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:42:16 AM,  12:25:13 PM, 0:42:57) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  12:13:37 PM,  12:30:00 PM, 0:16:23) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:24:22 AM,  11:26:31 AM, 0:02:09) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:16:24 AM,  12:30:00 PM, 1:13:36) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:01:15 AM,  11:01:32 AM, 0:00:17) \n (  11:01:32 AM,  12:24:32 PM, 1:23:00) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:59:35 AM,  12:02:09 PM, 0:02:34) \n (  12:02:53 PM,  12:30:00 PM, 0:27:07) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  10:59:29 AM,  11:02:18 AM, 0:02:49) \n (  11:17:23 AM,  12:25:50 PM, 1:08:27) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  10:56:32 AM,  10:59:04 AM, 0:02:32) \n (  10:59:05 AM,  12:25:13 PM, 1:26:08) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:07:05 AM,  12:01:45 PM, 0:54:40) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  10:58:54 AM,  10:59:04 AM, 0:00:10) \n (  10:59:05 AM,  12:18:38 PM, 1:19:33) \n (  12:22:20 PM,  12:30:00 PM, 0:07:40) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  10:57:44 AM,  10:59:04 AM, 0:01:20) \n (  10:59:06 AM,  11:36:12 AM, 0:37:06) \n (  11:37:03 AM,  12:26:07 PM, 0:49:04) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:12:09 AM,  11:36:04 AM, 0:23:55) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:01:23 AM,  12:30:00 PM, 1:28:37) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  10:57:51 AM,  10:58:22 AM, 0:00:31) \n (  10:58:57 AM,  10:59:03 AM, 0:00:06) \n (  10:59:05 AM,  12:25:48 PM, 1:26:43) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:01:42 AM,  11:01:49 AM, 0:00:07) \n (  11:03:06 AM,  11:03:13 AM, 0:00:07) \n (  11:04:26 AM,  11:31:12 AM, 0:26:46) \n (  11:32:21 AM,  12:21:46 PM, 0:49:25) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:08:35 AM,  12:24:27 PM, 1:15:52) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:00:01 AM,  11:00:06 AM, 0:00:05) \n (  11:00:22 AM,  12:25:36 PM, 1:25:14) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:50:48 AM,  12:13:12 PM, 0:22:24) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  10:56:12 AM,  10:56:16 AM, 0:00:04) \n (  11:01:29 AM,  11:01:37 AM, 0:00:08) \n (  11:03:05 AM,  11:03:11 AM, 0:00:06) \n (  11:15:20 AM,  12:16:00 PM, 1:00:40) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:00:09 AM,  11:02:57 AM, 0:02:48) \n (  11:03:32 AM,  12:25:07 PM, 1:21:35) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:51:10 AM,  12:24:55 PM, 0:33:45) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:11:17 AM,  12:04:07 PM, 0:52:50) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:07:51 AM,  12:25:13 PM, 1:17:22) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:00:14 AM,  12:30:00 PM, 1:29:46) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:16:55 AM,  11:48:32 AM, 0:31:37) \n (  11:48:46 AM,  11:49:33 AM, 0:00:47) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  10:56:12 AM,  10:56:34 AM, 0:00:22) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:02:03 AM,  12:30:00 PM, 1:27:57) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:04:31 AM,  11:04:45 AM, 0:00:14) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  10:57:08 AM,  10:59:05 AM, 0:01:57) \n (  10:59:05 AM,  12:21:52 PM, 1:22:47) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:05:59 AM,  11:06:25 AM, 0:00:26) \n (  11:06:40 AM,  11:51:48 AM, 0:45:08) \n (  11:57:55 AM,  12:30:00 PM, 0:32:05) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  12:21:14 PM,  12:25:10 PM, 0:03:56) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  10:57:44 AM,  10:59:04 AM, 0:01:20) \n (  10:59:04 AM,  11:55:52 AM, 0:56:48) \n (  11:59:19 AM,  12:24:53 PM, 0:25:34) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:32:42 AM,  12:24:26 PM, 0:51:44) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:06:32 AM,  11:23:56 AM, 0:17:24) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:02:11 AM,  12:30:00 PM, 1:27:49) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:01:49 AM,  11:01:58 AM, 0:00:09) \n (  11:01:58 AM,  11:03:24 AM, 0:01:26) \n (  11:03:28 AM,  12:25:03 PM, 1:21:35) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:31:47 AM,  11:41:58 AM, 0:10:11) \n (  11:59:31 AM,  12:04:22 PM, 0:04:51) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  10:59:31 AM,  12:25:00 PM, 1:25:29) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:00:46 AM,  12:24:38 PM, 1:23:52) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:11:15 AM,  12:30:00 PM, 1:18:45) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:01:01 AM,  11:01:13 AM, 0:00:12) \n (  11:01:13 AM,  12:24:29 PM, 1:23:16) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:16:33 AM,  11:18:41 AM, 0:02:08) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:00:22 AM,  12:24:41 PM, 1:24:19) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  10:59:19 AM,  12:24:23 PM, 1:25:04) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:00:31 AM,  11:47:23 AM, 0:46:52) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  10:56:12 AM,  10:59:03 AM, 0:02:51) \n (  10:57:29 AM,  10:59:05 AM, 0:01:36) \n (  10:59:04 AM,  11:37:00 AM, 0:37:56) \n (  10:59:06 AM,  12:25:18 PM, 1:26:12) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  10:56:12 AM,  12:25:15 PM, 1:29:03) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:06:11 AM,  12:05:09 PM, 0:58:58) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:01:34 AM,  11:12:49 AM, 0:11:15) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:45:23 AM,  12:25:08 PM, 0:39:45) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:00:09 AM,  12:25:02 PM, 1:24:53) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  10:56:14 AM,  10:56:21 AM, 0:00:07) \n (  10:59:45 AM,  11:00:21 AM, 0:00:36) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:00:37 AM,  11:01:15 AM, 0:00:38) \n (  11:01:15 AM,  11:23:00 AM, 0:21:45) \n (  12:12:13 PM,  12:22:38 PM, 0:10:25) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:02:06 AM,  12:25:00 PM, 1:22:54) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:19:57 AM,  11:21:25 AM, 0:01:28) \n (  11:24:00 AM,  12:25:03 PM, 1:01:03) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  10:56:14 AM,  10:59:06 AM, 0:02:52) \n (  10:59:07 AM,  11:59:05 AM, 0:59:58) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  10:59:53 AM,  12:25:04 PM, 1:25:11) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:02:49 AM,  11:03:24 AM, 0:00:35) \n (  11:03:24 AM,  12:24:58 PM, 1:21:34) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  10:57:56 AM,  10:59:07 AM, 0:01:11) \n (  10:59:07 AM,  12:24:36 PM, 1:25:29) \n (  11:34:46 AM,  12:27:15 PM, 0:52:29) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  10:57:39 AM,  10:59:07 AM, 0:01:28) \n (  10:59:07 AM,  12:24:36 PM, 1:25:29) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:21:29 AM,  12:24:58 PM, 1:03:29) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  10:59:25 AM,  12:17:44 PM, 1:18:19) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:02:34 AM,  11:34:36 AM, 0:32:02) \n (  11:35:02 AM,  12:25:04 PM, 0:50:02) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:26:42 AM,  12:25:05 PM, 0:58:23) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:00:44 AM,  11:01:14 AM, 0:00:30) \n (  11:01:14 AM,  11:21:55 AM, 0:20:41) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:04:26 AM,  11:04:35 AM, 0:00:09) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:02:49 AM,  12:24:58 PM, 1:22:09) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:05:04 AM,  11:05:46 AM, 0:00:42) \n (  11:05:46 AM,  12:30:00 PM, 1:24:14) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:20:41 AM,  11:23:17 AM, 0:02:36) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  10:59:13 AM,  10:59:21 AM, 0:00:08) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:24:21 AM,  12:24:59 PM, 1:00:38) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  10:58:03 AM,  10:58:08 AM, 0:00:05) \n (  10:59:07 AM,  12:24:52 PM, 1:25:45) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:32:38 AM,  12:25:02 PM, 0:52:24) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  10:56:12 AM,  10:57:10 AM, 0:00:58) \n (  11:00:13 AM,  12:14:51 PM, 1:14:38) \n (  12:16:25 PM,  12:30:00 PM, 0:13:35) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:08:45 AM,  11:14:40 AM, 0:05:55) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  10:58:43 AM,  10:59:04 AM, 0:00:21) \n (  10:59:05 AM,  12:25:10 PM, 1:26:05) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:35:43 AM,  12:23:35 PM, 0:47:52) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:13:09 AM,  11:50:42 AM, 0:37:33) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  10:57:37 AM,  10:59:03 AM, 0:01:26) \n (  10:59:04 AM,  12:30:00 PM, 1:30:56) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:02:33 AM,  12:24:56 PM, 1:22:23) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:00:51 AM,  12:25:04 PM, 1:24:13) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:06:52 AM,  12:25:05 PM, 1:18:13) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  10:57:47 AM,  10:58:09 AM, 0:00:22) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:01:49 AM,  11:37:50 AM, 0:36:01) \n (  11:38:00 AM,  12:16:12 PM, 0:38:12) \n (  12:17:57 PM,  12:25:14 PM, 0:07:17) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:09:46 AM,  11:46:00 AM, 0:36:14) \n (  11:46:14 AM,  12:25:16 PM, 0:39:02) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:05:06 AM,  12:24:57 PM, 1:19:51) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  10:58:49 AM,  10:59:05 AM, 0:00:16) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:13:00 AM,  11:15:15 AM, 0:02:15) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  12:22:04 PM,  12:24:57 PM, 0:02:53) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:01:57 AM,  11:37:08 AM, 0:35:11) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:08:28 AM,  12:24:45 PM, 1:16:17) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:07:24 AM,  11:56:41 AM, 0:49:17) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:02:14 AM,  12:25:03 PM, 1:22:49) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:00:01 AM,  11:05:38 AM, 0:05:37) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  10:56:12 AM,  12:25:05 PM, 1:28:53) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:00:27 AM,  11:01:14 AM, 0:00:47) \n (  11:01:14 AM,  12:25:06 PM, 1:23:52) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:07:16 AM,  11:15:45 AM, 0:08:29) \n (  11:16:35 AM,  12:25:01 PM, 1:08:26) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:40:22 AM,  11:41:35 AM, 0:01:13) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:01:33 AM,  12:03:59 PM, 1:02:26) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:00:08 AM,  12:27:30 PM, 1:27:22) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:01:47 AM,  12:24:35 PM, 1:22:48) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  10:56:53 AM,  10:57:01 AM, 0:00:08) \n (  10:57:07 AM,  10:59:05 AM, 0:01:58) \n (  10:58:40 AM,  10:59:05 AM, 0:00:25) \n (  10:59:06 AM,  11:00:25 AM, 0:01:19) \n (  11:01:08 AM,  12:26:59 PM, 1:25:51) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  10:58:27 AM,  10:58:52 AM, 0:00:25) \n (  11:00:32 AM,  12:30:00 PM, 1:29:28) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:15:27 AM,  12:25:13 PM, 1:09:46) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  10:56:16 AM,  10:59:05 AM, 0:02:49) \n (  10:59:06 AM,  12:24:58 PM, 1:25:52) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:03:01 AM,  12:26:57 PM, 1:23:56) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  10:58:58 AM,  10:59:33 AM, 0:00:35) \n (  11:00:30 AM,  12:03:51 PM, 1:03:21) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:14:25 AM,  11:20:25 AM, 0:06:00) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:03:40 AM,  12:14:23 PM, 1:10:43) \n (  12:14:30 PM,  12:25:04 PM, 0:10:34) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  10:59:47 AM,  11:00:02 AM, 0:00:15) \n (  11:00:02 AM,  12:25:12 PM, 1:25:10) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:11:30 AM,  12:09:29 PM, 0:57:59) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:07:40 AM,  12:30:00 PM, 1:22:20) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:00:05 AM,  12:15:24 PM, 1:15:19) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  10:58:08 AM,  10:59:05 AM, 0:00:57) \n (  10:59:06 AM,  12:24:29 PM, 1:25:23) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:10:35 AM,  12:25:16 PM, 1:14:41) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:04:00 AM,  11:04:13 AM, 0:00:13) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  10:59:12 AM,  11:16:55 AM, 0:17:43) \n (  11:17:42 AM,  12:24:01 PM, 1:06:19) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:27:38 AM,  11:28:47 AM, 0:01:09) \n (  11:30:34 AM,  11:44:52 AM, 0:14:18) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:02:43 AM,  11:02:59 AM, 0:00:16) \n (  11:03:19 AM,  12:25:01 PM, 1:21:42) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:55:42 AM,  11:58:13 AM, 0:02:31) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:04:42 AM,  11:04:59 AM, 0:00:17) \n (  11:04:59 AM,  11:05:34 AM, 0:00:35) \n (  11:07:32 AM,  11:12:04 AM, 0:04:32) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:05:07 AM,  11:14:35 AM, 0:09:28) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:16:44 AM,  11:45:33 AM, 0:28:49) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  10:56:12 AM,  12:25:10 PM, 1:28:58) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  10:56:19 AM,  12:25:34 PM, 1:29:15) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:03:54 AM,  12:23:36 PM, 1:19:42) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:56:03 AM,  12:06:08 PM, 0:10:05) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:00:47 AM,  11:01:11 AM, 0:00:24) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:12:32 AM,  12:03:03 PM, 0:50:31) \n (  12:04:41 PM,  12:11:01 PM, 0:06:20) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:01:03 AM,  11:05:09 AM, 0:04:06) \n (  11:05:12 AM,  11:07:02 AM, 0:01:50) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:45:53 AM,  11:48:00 AM, 0:02:07) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:01:44 AM,  12:16:50 PM, 1:15:06) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:07:04 AM,  12:24:40 PM, 1:17:36) \n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(  11:01:17 AM,  11:03:05 AM, 0:01:48) \n (  11:02:50 AM,  11:03:22 AM, 0:00:32) \n (  11:03:22 AM,  11:07:12 AM, 0:03:50) \n (  11:06:27 AM,  12:15:03 PM, 1:08:36) \n (  12:13:07 PM,  12:25:08 PM, 0:12:01) \n </t>
   </si>
   <si>
     <t>Present</t>

</xml_diff>